<commit_message>
Answer questions in SIQ sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/SIQ/PO2EBL_SIQ.xlsx
+++ b/SW deliveries log/SIQ/PO2EBL_SIQ.xlsx
@@ -168,6 +168,7 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -323,10 +324,10 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.86"/>

</xml_diff>

<commit_message>
update the folder structure
Signed-off-by: Mohammmedibra96 <mohammedibra96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/SIQ/PO2EBL_SIQ.xlsx
+++ b/SW deliveries log/SIQ/PO2EBL_SIQ.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\software\project\SW deliveries log\SIQ\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,69 +24,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">REQ_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asked by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+  <si>
+    <t>REQ_ID</t>
+  </si>
+  <si>
+    <t>Asked by</t>
+  </si>
+  <si>
+    <t>SIQ_ID</t>
   </si>
   <si>
     <t xml:space="preserve">Question
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Proposed Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected Response date</t>
+    <t>Proposed Answer</t>
+  </si>
+  <si>
+    <t>Sub date</t>
+  </si>
+  <si>
+    <t>Expected Response date</t>
   </si>
   <si>
     <t xml:space="preserve">Response date
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mohamed Ibrahim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regarding budget, we have AVR uc for 50 LE and STM for 110LE, which one do you prefer?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We recommend the AVR to meet budget limitations as we don't need the extra capabilities of the STM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/1/2020</t>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Mohamed Ibrahim</t>
+  </si>
+  <si>
+    <t>Regarding budget, we have AVR uc for 50 LE and STM for 110LE, which one do you prefer?</t>
+  </si>
+  <si>
+    <t>We recommend the AVR to meet budget limitations as we don't need the extra capabilities of the STM</t>
+  </si>
+  <si>
+    <t>22/1/2020</t>
   </si>
   <si>
     <t xml:space="preserve">
 22/1/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">27/1/2020</t>
+    <t>27/1/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Use AVR uc. </t>
   </si>
   <si>
-    <t xml:space="preserve">Mohamed Farag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are the propesed duty cycle for the Speeds?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed 1: 30% 
+    <t>Mohamed Farag</t>
+  </si>
+  <si>
+    <t>What are the propesed duty cycle for the Speeds?</t>
+  </si>
+  <si>
+    <t>Speed 1: 30% 
 Speed 2: 60% 
 Speed 3: 90%</t>
   </si>
@@ -91,12 +95,12 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Speed 1 : from 0% up to 30%. 
+    <t>Speed 1 : from 0% up to 30%. 
 Speed 2: above 30% up to 60%. 
 Speed 3: above  60 % up to 100%.</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you need a speed indicator for the blender?</t>
+    <t>Do you need a speed indicator for the blender?</t>
   </si>
   <si>
     <t xml:space="preserve">LEDs or LCD 
@@ -114,60 +118,41 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">What is the proposed motor power? (essential for blender performance)</t>
+    <t>What is the proposed motor power? (essential for blender performance)</t>
   </si>
   <si>
     <t xml:space="preserve">Pick up any model of DC motor which delivers a sufficient power for Electric Blender. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">accepted </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -186,7 +171,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -194,65 +179,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -311,31 +261,305 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
+    <col min="4" max="4" width="50.90625" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="8" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +592,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -392,9 +616,11 @@
       <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="85.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="112" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
@@ -418,9 +644,11 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="98" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -444,9 +672,11 @@
       <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="112" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -468,9 +698,11 @@
       <c r="I5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -482,7 +714,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -494,7 +726,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -506,7 +738,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -518,7 +750,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -530,7 +762,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -542,7 +774,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -554,7 +786,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -566,7 +798,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -578,7 +810,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -590,7 +822,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -602,7 +834,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -614,7 +846,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -626,7 +858,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -638,7 +870,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -650,7 +882,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -662,7 +894,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -674,7 +906,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -686,7 +918,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -698,7 +930,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -710,7 +942,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -722,7 +954,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -734,7 +966,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -746,7 +978,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -758,7 +990,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -770,7 +1002,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -783,12 +1015,7 @@
       <c r="J31" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>